<commit_message>
Removing Pivot-Cache feature for Calling Fn (#10)
* removing feature for pivot-cache and replacing with calling fn

* simplifying & correcting access to PivotDataRef by index.

---------

Co-authored-by: GitHub Actions <actions@github.com>
</commit_message>
<xml_diff>
--- a/tests/pivots.xlsx
+++ b/tests/pivots.xlsx
@@ -5,22 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelgilmore/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelgilmore/Code/calamine/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22403EC8-C91A-5941-B084-8AD0990BE76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F20162-1C5A-824E-8AA1-05ED4117733A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19160" yWindow="3260" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{B0C1159D-33EE-DB47-84B2-FAAEB7E2FFDF}"/>
+    <workbookView xWindow="19160" yWindow="3260" windowWidth="28040" windowHeight="17440" xr2:uid="{B0C1159D-33EE-DB47-84B2-FAAEB7E2FFDF}"/>
   </bookViews>
   <sheets>
     <sheet name="PivotSheet1" sheetId="2" r:id="rId1"/>
     <sheet name="PivotSheet2" sheetId="3" r:id="rId2"/>
     <sheet name="PivotSheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="DataSheet" sheetId="1" r:id="rId4"/>
+    <sheet name="PivotSheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="DataSheet" sheetId="1" r:id="rId5"/>
+    <sheet name="DataSheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="89" r:id="rId5"/>
+    <pivotCache cacheId="65" r:id="rId7"/>
+    <pivotCache cacheId="64" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -154,6 +157,9 @@
   </si>
   <si>
     <t>&lt;--------  grouped field as value</t>
+  </si>
+  <si>
+    <t>Sum of Value</t>
   </si>
 </sst>
 </file>
@@ -318,6 +324,54 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="joel gilmore" refreshedDate="45985.414996412037" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="10" xr:uid="{823ACCA9-2AA8-E746-A301-4BC8322E99F8}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:J11" sheet="DataSheet2"/>
+  </cacheSource>
+  <cacheFields count="10">
+    <cacheField name="Id" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
+    </cacheField>
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems count="2">
+        <s v="blue"/>
+        <s v="yellow"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Value" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="20"/>
+    </cacheField>
+    <cacheField name="Size" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="4.0309999999999997"/>
+    </cacheField>
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1999-01-01T00:00:00" maxDate="2024-12-02T00:00:00"/>
+    </cacheField>
+    <cacheField name="Value / Size" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="1.2403870007442324" maxValue="14.394012090970156"/>
+    </cacheField>
+    <cacheField name="IsBlue" numFmtId="14">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Null" numFmtId="14">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Misc" numFmtId="0">
+      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2024-02-01T00:00:00" maxDate="1899-12-31T00:53:04"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="10">
   <r>
@@ -443,8 +497,133 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="10">
+  <r>
+    <n v="1"/>
+    <s v="a"/>
+    <x v="0"/>
+    <n v="20"/>
+    <n v="1.78"/>
+    <d v="2024-11-01T00:00:00"/>
+    <n v="11.235955056179774"/>
+    <b v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="b"/>
+    <x v="0"/>
+    <n v="20"/>
+    <n v="2.012"/>
+    <d v="2024-01-04T00:00:00"/>
+    <n v="9.9403578528827037"/>
+    <b v="1"/>
+    <m/>
+    <n v="2.012"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="c"/>
+    <x v="0"/>
+    <n v="20"/>
+    <n v="3.121"/>
+    <d v="2024-01-31T00:00:00"/>
+    <n v="6.4082024991989748"/>
+    <b v="1"/>
+    <m/>
+    <d v="2024-02-01T00:00:00"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="d"/>
+    <x v="0"/>
+    <n v="10"/>
+    <n v="1.052"/>
+    <d v="2024-01-21T00:00:00"/>
+    <n v="9.5057034220532319"/>
+    <b v="1"/>
+    <m/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <s v="e"/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="3.1019999999999999"/>
+    <d v="2024-02-01T00:00:00"/>
+    <n v="1.6118633139909737"/>
+    <b v="1"/>
+    <m/>
+    <n v="3.1019999999999999"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="f"/>
+    <x v="1"/>
+    <n v="10"/>
+    <n v="1.02"/>
+    <d v="2024-01-01T00:00:00"/>
+    <n v="9.8039215686274517"/>
+    <b v="0"/>
+    <m/>
+    <n v="20"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <s v="g"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="0"/>
+    <d v="2024-01-11T00:00:00"/>
+    <e v="#DIV/0!"/>
+    <b v="0"/>
+    <m/>
+    <b v="1"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="h"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="4.0309999999999997"/>
+    <d v="1999-01-01T00:00:00"/>
+    <n v="1.2403870007442324"/>
+    <b v="0"/>
+    <m/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <s v="i"/>
+    <x v="1"/>
+    <n v="15"/>
+    <n v="1.0421"/>
+    <d v="2024-12-01T00:00:00"/>
+    <n v="14.394012090970156"/>
+    <b v="0"/>
+    <m/>
+    <n v="10"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <s v="j"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="1.20452"/>
+    <d v="2024-01-01T00:00:00"/>
+    <n v="4.1510311161292464"/>
+    <b v="0"/>
+    <m/>
+    <s v="blue"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55812D53-A4C4-8C41-92AB-7401E334F510}" name="PivotTable1" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55812D53-A4C4-8C41-92AB-7401E334F510}" name="PivotTable1" cacheId="65" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -543,7 +722,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B2EEFC0A-A4C8-3849-8A15-494E25A1739B}" name="PivotTable2" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B2EEFC0A-A4C8-3849-8A15-494E25A1739B}" name="PivotTable2" cacheId="65" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -653,7 +832,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0BD01C9-9EE0-7246-B5FE-6615AC2FE614}" name="PivotTable1" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0BD01C9-9EE0-7246-B5FE-6615AC2FE614}" name="PivotTable1" cacheId="65" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -755,6 +934,127 @@
   </pageFields>
   <dataFields count="1">
     <dataField name="Count of Value2" fld="11" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EE27EDA5-4AA7-E94E-8CA2-EECF7E18E7ED}" name="PivotTable6" cacheId="65" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A6:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD472F44-EE1F-C542-B642-A08CF695847D}" name="PivotTable5" cacheId="64" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1067,8 +1367,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CDD472D-C7DD-5A4C-BF76-DA38C4FDEA79}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pivotSelection pane="bottomRight" click="1" r:id="rId1">
+        <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1291,7 +1593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6AFD90-4D9E-104E-B9F0-279E16F38CB4}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1334,7 +1636,7 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -1342,7 +1644,7 @@
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
@@ -1350,7 +1652,7 @@
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
@@ -1358,7 +1660,7 @@
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>3</v>
       </c>
     </row>
@@ -1368,11 +1670,94 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8864F807-C779-854C-AEC1-C4BCC91C0FED}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0755B1D2-8DC8-E04D-888E-19765C24246D}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection sqref="A1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1647,6 +2032,362 @@
       <c r="G9">
         <f t="shared" si="0"/>
         <v>3.7211610022326971</v>
+      </c>
+      <c r="H9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>1.0421</v>
+      </c>
+      <c r="F10" s="3">
+        <v>45627</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>14.394012090970156</v>
+      </c>
+      <c r="H10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>1.20452</v>
+      </c>
+      <c r="F11" s="3">
+        <v>45292</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>4.1510311161292464</v>
+      </c>
+      <c r="H11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1DD2E4-F94F-1245-BFED-8EFC70543B88}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>1.78</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45597</v>
+      </c>
+      <c r="G2">
+        <f>D2/E2</f>
+        <v>11.235955056179774</v>
+      </c>
+      <c r="H2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>2.012</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45295</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G11" si="0">D3/E3</f>
+        <v>9.9403578528827037</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3">
+        <v>2.012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>3.121</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45322</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>6.4082024991989748</v>
+      </c>
+      <c r="H4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>1.052</v>
+      </c>
+      <c r="F5" s="3">
+        <v>45312</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>9.5057034220532319</v>
+      </c>
+      <c r="H5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>3.1019999999999999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>45323</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1.6118633139909737</v>
+      </c>
+      <c r="H6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6">
+        <v>3.1019999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>1.02</v>
+      </c>
+      <c r="F7" s="3">
+        <v>45292</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>9.8039215686274517</v>
+      </c>
+      <c r="H7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>45302</v>
+      </c>
+      <c r="G8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>4.0309999999999997</v>
+      </c>
+      <c r="F9" s="3">
+        <v>36161</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1.2403870007442324</v>
       </c>
       <c r="H9" s="3" t="b">
         <v>0</v>

</xml_diff>